<commit_message>
ran pcangsd on n-amer-no-clones
</commit_message>
<xml_diff>
--- a/data/01_pd-samples/25_12-01_pd_samples-edited.xlsx
+++ b/data/01_pd-samples/25_12-01_pd_samples-edited.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/caprinapugliese/Documents/School/Uconn/2024-26_Grad_School/Dagilis-lab/WNS-project/data/01_pd-samples/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE49053A-6670-5549-981D-F056B45D3398}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93D4AA0C-F894-5D47-867C-36BCB89380BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4760" yWindow="1120" windowWidth="31740" windowHeight="18680" xr2:uid="{D99E271A-162C-F24C-8D0E-BBA6ED327C07}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1046" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1049" uniqueCount="420">
   <si>
     <t>sample_id</t>
   </si>
@@ -1291,6 +1291,9 @@
   </si>
   <si>
     <t>https://www.nps.gov/articles/000/bats-in-acadia-facing-challenges-but-hanging-on.htm &lt;-- good article on bats in acadia national park</t>
+  </si>
+  <si>
+    <t>Pd_N. American</t>
   </si>
 </sst>
 </file>
@@ -2250,8 +2253,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4D9535-1238-AB48-B467-419735026371}">
   <dimension ref="A1:X75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B49" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E71" sqref="E71"/>
+    <sheetView tabSelected="1" topLeftCell="C44" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="V70" sqref="V70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4588,107 +4591,92 @@
         <v>307</v>
       </c>
     </row>
-    <row r="42" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>126</v>
-      </c>
-      <c r="B42" s="7" t="s">
-        <v>127</v>
-      </c>
-      <c r="C42" s="7" t="s">
-        <v>126</v>
+        <v>85</v>
+      </c>
+      <c r="B42" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" t="s">
+        <v>85</v>
       </c>
       <c r="D42" s="5">
-        <v>1955487</v>
+        <v>5755629</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>128</v>
+        <v>87</v>
       </c>
       <c r="F42" t="s">
         <v>51</v>
       </c>
       <c r="G42" t="s">
-        <v>129</v>
+        <v>88</v>
       </c>
       <c r="H42">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="I42">
-        <v>2008</v>
+        <v>2009</v>
       </c>
       <c r="J42" t="s">
-        <v>130</v>
+        <v>42</v>
       </c>
       <c r="K42" t="s">
         <v>43</v>
       </c>
-      <c r="L42" t="s">
-        <v>20</v>
+      <c r="L42" s="10" t="s">
+        <v>25</v>
       </c>
       <c r="M42" t="s">
-        <v>298</v>
+        <v>323</v>
       </c>
       <c r="N42" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="O42" t="s">
         <v>305</v>
       </c>
-      <c r="P42" t="s">
-        <v>394</v>
-      </c>
       <c r="Q42">
-        <v>43.835385505600499</v>
+        <v>50.788476564399403</v>
       </c>
       <c r="R42">
-        <v>-92.283091749633499</v>
-      </c>
-      <c r="S42" t="s">
-        <v>379</v>
-      </c>
-      <c r="T42" t="s">
-        <v>380</v>
+        <v>10.740499703414899</v>
       </c>
       <c r="U42" t="s">
-        <v>378</v>
-      </c>
-      <c r="V42" s="7" t="s">
-        <v>397</v>
-      </c>
-      <c r="W42" s="6" t="s">
-        <v>386</v>
-      </c>
-    </row>
-    <row r="43" spans="1:24" ht="51" x14ac:dyDescent="0.2">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="43" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C43" s="7" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="D43" s="5">
-        <v>1955239</v>
+        <v>1955487</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F43" t="s">
         <v>51</v>
       </c>
       <c r="G43" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H43">
-        <v>1960</v>
+        <v>2008</v>
       </c>
       <c r="I43">
-        <v>1960</v>
+        <v>2008</v>
       </c>
       <c r="J43" t="s">
-        <v>117</v>
+        <v>130</v>
       </c>
       <c r="K43" t="s">
         <v>43</v>
@@ -4700,19 +4688,19 @@
         <v>298</v>
       </c>
       <c r="N43" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="O43" t="s">
         <v>305</v>
       </c>
       <c r="P43" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="Q43">
-        <v>45.876656556660201</v>
+        <v>43.835385505600499</v>
       </c>
       <c r="R43">
-        <v>-89.628365849641099</v>
+        <v>-92.283091749633499</v>
       </c>
       <c r="S43" t="s">
         <v>379</v>
@@ -4724,42 +4712,39 @@
         <v>378</v>
       </c>
       <c r="V43" s="7" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="W43" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="X43" s="2" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="44" spans="1:24" ht="17" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:24" ht="51" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C44" s="7" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D44" s="5">
-        <v>1955482</v>
+        <v>1955239</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="F44" t="s">
         <v>51</v>
       </c>
       <c r="G44" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="H44">
-        <v>2002</v>
+        <v>1960</v>
       </c>
       <c r="I44">
-        <v>2002</v>
+        <v>1960</v>
       </c>
       <c r="J44" t="s">
         <v>117</v>
@@ -4771,22 +4756,22 @@
         <v>20</v>
       </c>
       <c r="M44" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N44" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="O44" t="s">
         <v>305</v>
       </c>
       <c r="P44" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="Q44">
-        <v>53.933300000000003</v>
+        <v>45.876656556660201</v>
       </c>
       <c r="R44">
-        <v>-116.5765</v>
+        <v>-89.628365849641099</v>
       </c>
       <c r="S44" t="s">
         <v>379</v>
@@ -4798,39 +4783,42 @@
         <v>378</v>
       </c>
       <c r="V44" s="7" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="W44" s="6" t="s">
         <v>386</v>
       </c>
+      <c r="X44" s="2" t="s">
+        <v>404</v>
+      </c>
     </row>
     <row r="45" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C45" s="7" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="D45" s="5">
-        <v>1955483</v>
+        <v>1955482</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="F45" t="s">
         <v>51</v>
       </c>
       <c r="G45" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="H45">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="I45">
-        <v>2008</v>
+        <v>2002</v>
       </c>
       <c r="J45" t="s">
         <v>117</v>
@@ -4842,22 +4830,22 @@
         <v>20</v>
       </c>
       <c r="M45" t="s">
-        <v>298</v>
+        <v>291</v>
       </c>
       <c r="N45" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="O45" t="s">
         <v>305</v>
       </c>
       <c r="P45" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="Q45">
-        <v>42.871989999999997</v>
+        <v>53.933300000000003</v>
       </c>
       <c r="R45">
-        <v>-73.226607000000001</v>
+        <v>-116.5765</v>
       </c>
       <c r="S45" t="s">
         <v>379</v>
@@ -4869,7 +4857,7 @@
         <v>378</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="W45" s="6" t="s">
         <v>386</v>
@@ -4877,25 +4865,25 @@
     </row>
     <row r="46" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C46" s="7" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D46" s="5">
-        <v>1955484</v>
+        <v>1955483</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="F46" t="s">
         <v>51</v>
       </c>
       <c r="G46" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="H46">
         <v>2008</v>
@@ -4916,7 +4904,7 @@
         <v>298</v>
       </c>
       <c r="N46" t="s">
-        <v>299</v>
+        <v>304</v>
       </c>
       <c r="O46" t="s">
         <v>305</v>
@@ -4925,10 +4913,10 @@
         <v>394</v>
       </c>
       <c r="Q46">
-        <v>41.844515371877698</v>
+        <v>42.871989999999997</v>
       </c>
       <c r="R46">
-        <v>-74.098548155198898</v>
+        <v>-73.226607000000001</v>
       </c>
       <c r="S46" t="s">
         <v>379</v>
@@ -4940,7 +4928,7 @@
         <v>378</v>
       </c>
       <c r="V46" s="7" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="W46" s="6" t="s">
         <v>386</v>
@@ -4948,25 +4936,25 @@
     </row>
     <row r="47" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="C47" s="7" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D47" s="5">
-        <v>1955485</v>
+        <v>1955484</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="F47" t="s">
         <v>51</v>
       </c>
       <c r="G47" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="H47">
         <v>2008</v>
@@ -4987,19 +4975,19 @@
         <v>298</v>
       </c>
       <c r="N47" t="s">
-        <v>302</v>
+        <v>299</v>
       </c>
       <c r="O47" t="s">
         <v>305</v>
       </c>
-      <c r="P47" s="2" t="s">
-        <v>407</v>
+      <c r="P47" t="s">
+        <v>394</v>
       </c>
       <c r="Q47">
-        <v>45.876656556660201</v>
+        <v>41.844515371877698</v>
       </c>
       <c r="R47">
-        <v>-89.628365849641099</v>
+        <v>-74.098548155198898</v>
       </c>
       <c r="S47" t="s">
         <v>379</v>
@@ -5011,7 +4999,7 @@
         <v>378</v>
       </c>
       <c r="V47" s="7" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="W47" s="6" t="s">
         <v>386</v>
@@ -5019,25 +5007,25 @@
     </row>
     <row r="48" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C48" s="7" t="s">
-        <v>126</v>
+        <v>147</v>
       </c>
       <c r="D48" s="5">
-        <v>1955486</v>
+        <v>1955485</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="F48" t="s">
         <v>51</v>
       </c>
       <c r="G48" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="H48">
         <v>2008</v>
@@ -5046,10 +5034,10 @@
         <v>2008</v>
       </c>
       <c r="J48" t="s">
-        <v>18</v>
+        <v>117</v>
       </c>
       <c r="K48" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="L48" t="s">
         <v>20</v>
@@ -5058,19 +5046,19 @@
         <v>298</v>
       </c>
       <c r="N48" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="O48" t="s">
         <v>305</v>
       </c>
-      <c r="P48" t="s">
-        <v>394</v>
+      <c r="P48" s="2" t="s">
+        <v>407</v>
       </c>
       <c r="Q48">
-        <v>43.835385505600499</v>
+        <v>45.876656556660201</v>
       </c>
       <c r="R48">
-        <v>-92.283091749633499</v>
+        <v>-89.628365849641099</v>
       </c>
       <c r="S48" t="s">
         <v>379</v>
@@ -5082,95 +5070,113 @@
         <v>378</v>
       </c>
       <c r="V48" s="7" t="s">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="W48" s="6" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="49" spans="1:24" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:24" ht="17" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>138</v>
-      </c>
-      <c r="B49" t="s">
-        <v>227</v>
-      </c>
-      <c r="C49" t="s">
-        <v>138</v>
+        <v>126</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>126</v>
       </c>
       <c r="D49" s="5">
-        <v>6011483</v>
+        <v>1955486</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>228</v>
+        <v>152</v>
       </c>
       <c r="F49" t="s">
         <v>51</v>
       </c>
       <c r="G49" t="s">
-        <v>229</v>
+        <v>153</v>
       </c>
       <c r="H49">
-        <v>2010</v>
-      </c>
-      <c r="I49" s="1">
-        <v>40252</v>
+        <v>2008</v>
+      </c>
+      <c r="I49">
+        <v>2008</v>
       </c>
       <c r="J49" t="s">
-        <v>130</v>
+        <v>18</v>
       </c>
       <c r="K49" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="L49" t="s">
         <v>20</v>
       </c>
       <c r="M49" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="N49" t="s">
-        <v>319</v>
+        <v>301</v>
       </c>
       <c r="O49" t="s">
         <v>305</v>
       </c>
+      <c r="P49" t="s">
+        <v>394</v>
+      </c>
       <c r="Q49">
-        <v>48.174337000000001</v>
+        <v>43.835385505600499</v>
       </c>
       <c r="R49">
-        <v>80.100126000000003</v>
+        <v>-92.283091749633499</v>
+      </c>
+      <c r="S49" t="s">
+        <v>379</v>
+      </c>
+      <c r="T49" t="s">
+        <v>380</v>
+      </c>
+      <c r="U49" t="s">
+        <v>378</v>
+      </c>
+      <c r="V49" s="7" t="s">
+        <v>397</v>
+      </c>
+      <c r="W49" s="6" t="s">
+        <v>386</v>
       </c>
     </row>
     <row r="50" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="B50" t="s">
-        <v>86</v>
+        <v>169</v>
       </c>
       <c r="C50" t="s">
-        <v>85</v>
+        <v>168</v>
       </c>
       <c r="D50" s="5">
-        <v>5755629</v>
+        <v>6011467</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>87</v>
+        <v>170</v>
       </c>
       <c r="F50" t="s">
         <v>51</v>
       </c>
       <c r="G50" t="s">
-        <v>88</v>
+        <v>171</v>
       </c>
       <c r="H50">
         <v>2009</v>
       </c>
-      <c r="I50">
-        <v>2009</v>
+      <c r="I50" s="1">
+        <v>39879</v>
       </c>
       <c r="J50" t="s">
-        <v>42</v>
+        <v>130</v>
       </c>
       <c r="K50" t="s">
         <v>43</v>
@@ -5193,37 +5199,37 @@
       <c r="R50">
         <v>10.740499703414899</v>
       </c>
-      <c r="U50" t="s">
-        <v>325</v>
+      <c r="X50" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="51" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="B51" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="C51" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="D51" s="5">
-        <v>6011467</v>
+        <v>6011468</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="F51" t="s">
         <v>51</v>
       </c>
       <c r="G51" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="H51">
         <v>2009</v>
       </c>
       <c r="I51" s="1">
-        <v>39879</v>
+        <v>39904</v>
       </c>
       <c r="J51" t="s">
         <v>130</v>
@@ -5235,19 +5241,19 @@
         <v>25</v>
       </c>
       <c r="M51" t="s">
-        <v>323</v>
+        <v>336</v>
       </c>
       <c r="N51" t="s">
-        <v>324</v>
+        <v>338</v>
       </c>
       <c r="O51" t="s">
         <v>305</v>
       </c>
       <c r="Q51">
-        <v>50.788476564399403</v>
+        <v>47.083329999999997</v>
       </c>
       <c r="R51">
-        <v>10.740499703414899</v>
+        <v>8</v>
       </c>
       <c r="X51" t="s">
         <v>26</v>
@@ -5255,31 +5261,31 @@
     </row>
     <row r="52" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
       <c r="B52" t="s">
-        <v>172</v>
+        <v>210</v>
       </c>
       <c r="C52" t="s">
-        <v>171</v>
+        <v>209</v>
       </c>
       <c r="D52" s="5">
-        <v>6011468</v>
+        <v>6011465</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>173</v>
+        <v>211</v>
       </c>
       <c r="F52" t="s">
         <v>51</v>
       </c>
       <c r="G52" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="H52">
         <v>2009</v>
       </c>
       <c r="I52" s="1">
-        <v>39904</v>
+        <v>39901</v>
       </c>
       <c r="J52" t="s">
         <v>130</v>
@@ -5291,19 +5297,19 @@
         <v>25</v>
       </c>
       <c r="M52" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="N52" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="O52" t="s">
         <v>305</v>
       </c>
       <c r="Q52">
-        <v>47.083329999999997</v>
+        <v>47.145499999999998</v>
       </c>
       <c r="R52">
-        <v>8</v>
+        <v>17.622399999999999</v>
       </c>
       <c r="X52" t="s">
         <v>26</v>
@@ -5311,31 +5317,31 @@
     </row>
     <row r="53" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="B53" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="C53" t="s">
-        <v>209</v>
+        <v>138</v>
       </c>
       <c r="D53" s="5">
-        <v>6011465</v>
+        <v>6011483</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="F53" t="s">
         <v>51</v>
       </c>
       <c r="G53" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="H53">
-        <v>2009</v>
+        <v>2010</v>
       </c>
       <c r="I53" s="1">
-        <v>39901</v>
+        <v>40252</v>
       </c>
       <c r="J53" t="s">
         <v>130</v>
@@ -5343,26 +5349,23 @@
       <c r="K53" t="s">
         <v>43</v>
       </c>
-      <c r="L53" s="10" t="s">
-        <v>25</v>
+      <c r="L53" t="s">
+        <v>20</v>
       </c>
       <c r="M53" t="s">
-        <v>335</v>
+        <v>291</v>
       </c>
       <c r="N53" t="s">
-        <v>337</v>
+        <v>319</v>
       </c>
       <c r="O53" t="s">
         <v>305</v>
       </c>
       <c r="Q53">
-        <v>47.145499999999998</v>
+        <v>48.174337000000001</v>
       </c>
       <c r="R53">
-        <v>17.622399999999999</v>
-      </c>
-      <c r="X53" t="s">
-        <v>26</v>
+        <v>80.100126000000003</v>
       </c>
     </row>
     <row r="54" spans="1:24" x14ac:dyDescent="0.2">
@@ -6257,14 +6260,23 @@
       <c r="O69" t="s">
         <v>300</v>
       </c>
+      <c r="P69" t="s">
+        <v>406</v>
+      </c>
       <c r="Q69">
         <v>41.844515371877698</v>
       </c>
       <c r="R69">
         <v>-74.098548155198898</v>
       </c>
+      <c r="S69" t="s">
+        <v>415</v>
+      </c>
       <c r="U69" t="s">
         <v>325</v>
+      </c>
+      <c r="V69" t="s">
+        <v>419</v>
       </c>
     </row>
     <row r="70" spans="1:24" ht="51" x14ac:dyDescent="0.2">
@@ -6683,7 +6695,7 @@
     <hyperlink ref="W70" r:id="rId3" xr:uid="{FF3869F2-7E6B-564D-B22A-72301C0CD2D9}"/>
     <hyperlink ref="W7:W13" r:id="rId4" display="https://doi.org/10.1038/s41467-017-02441-z" xr:uid="{FE3B581E-1BDF-7147-B4C6-D87A8EF543CC}"/>
     <hyperlink ref="W22" r:id="rId5" xr:uid="{0CBBFC48-3FDD-3848-9FEF-469016A3D5BA}"/>
-    <hyperlink ref="W43" r:id="rId6" xr:uid="{F8807A9D-D241-9243-BABA-D5FFA95D12B7}"/>
+    <hyperlink ref="W44" r:id="rId6" xr:uid="{F8807A9D-D241-9243-BABA-D5FFA95D12B7}"/>
     <hyperlink ref="W2" r:id="rId7" xr:uid="{EC6F4932-8C94-F740-9969-1B4806139AE2}"/>
     <hyperlink ref="W24" r:id="rId8" xr:uid="{CD5A617C-B212-8841-BF6B-C6AF934AFEB4}"/>
     <hyperlink ref="W3" r:id="rId9" xr:uid="{E51461B0-4697-2E4B-923D-E3A487F55731}"/>

</xml_diff>